<commit_message>
imprementando a listagem de algumas actions
</commit_message>
<xml_diff>
--- a/tarefas.xlsx
+++ b/tarefas.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lilia\Desktop\LABENGENHARIA\quizz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caique.fagundes\Desktop\projeto\quizz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CEE7F3-CB5F-4F73-9CC8-23312B9B6597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397E66ED-924A-46DA-A4E2-E35BA7EC7879}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56AB0845-96B2-4058-8F7F-7188F6E2D689}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{56AB0845-96B2-4058-8F7F-7188F6E2D689}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="66">
   <si>
     <t>acesso</t>
   </si>
@@ -216,13 +214,28 @@
   </si>
   <si>
     <t>listar partidas</t>
+  </si>
+  <si>
+    <t>TRABALHADOR</t>
+  </si>
+  <si>
+    <t>FEITO</t>
+  </si>
+  <si>
+    <t>LILIAN</t>
+  </si>
+  <si>
+    <t>CAIQUE</t>
+  </si>
+  <si>
+    <t>REALIZADO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,13 +243,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -251,8 +292,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,35 +624,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B6ACCB9-7BCF-486E-B701-AF27BF570F5B}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -608,8 +673,12 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -622,8 +691,12 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -636,8 +709,14 @@
       <c r="D4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -650,8 +729,10 @@
       <c r="D5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="2"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -664,8 +745,14 @@
       <c r="D6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -678,8 +765,11 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" s="2"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -692,8 +782,19 @@
       <c r="D8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9" s="2"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -706,8 +807,14 @@
       <c r="D10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -720,8 +827,10 @@
       <c r="D11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F11" s="1"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -734,8 +843,12 @@
       <c r="D12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -748,8 +861,12 @@
       <c r="D13" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -762,8 +879,12 @@
       <c r="D14" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -776,8 +897,12 @@
       <c r="D15" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -790,8 +915,12 @@
       <c r="D16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -804,8 +933,14 @@
       <c r="D17" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -818,8 +953,12 @@
       <c r="D18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -832,8 +971,12 @@
       <c r="D19" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -846,8 +989,14 @@
       <c r="D20" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -860,8 +1009,16 @@
       <c r="D21" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="2"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -874,8 +1031,10 @@
       <c r="D23" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="2"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -888,8 +1047,10 @@
       <c r="D24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="2"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -902,8 +1063,10 @@
       <c r="D25" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="2"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -916,8 +1079,10 @@
       <c r="D26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="2"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -930,8 +1095,10 @@
       <c r="D27" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27" s="2"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -944,8 +1111,12 @@
       <c r="D28" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -958,8 +1129,16 @@
       <c r="D29" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E30" s="2"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -972,8 +1151,12 @@
       <c r="D31" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -986,8 +1169,12 @@
       <c r="D32" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -1000,8 +1187,32 @@
       <c r="D33" t="s">
         <v>60</v>
       </c>
+      <c r="E33" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E34" s="2"/>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E35" s="2"/>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E36" s="2"/>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E37" s="2"/>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
aplicando formulário de sugestão
</commit_message>
<xml_diff>
--- a/tarefas.xlsx
+++ b/tarefas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caique.fagundes\Desktop\projeto\quizz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397E66ED-924A-46DA-A4E2-E35BA7EC7879}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7D3134-85B0-4FC8-8FF0-F6E6178F8308}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{56AB0845-96B2-4058-8F7F-7188F6E2D689}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="66">
   <si>
     <t>acesso</t>
   </si>
@@ -627,7 +627,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,7 +1012,9 @@
       <c r="E21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E22" s="2"/>
@@ -1114,7 +1116,9 @@
       <c r="E28" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="1"/>
+      <c r="F28" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1132,7 +1136,9 @@
       <c r="E29" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F29" s="1"/>
+      <c r="F29" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E30" s="2"/>

</xml_diff>

<commit_message>
login com retorno de usuario adm e user
</commit_message>
<xml_diff>
--- a/tarefas.xlsx
+++ b/tarefas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caique.fagundes\Desktop\projeto\quizz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lilia\Desktop\LABENGENHARIA\quizz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7D3134-85B0-4FC8-8FF0-F6E6178F8308}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E54F6F-0F48-463E-98DC-6229C430B831}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{56AB0845-96B2-4058-8F7F-7188F6E2D689}"/>
+    <workbookView xWindow="-38520" yWindow="0" windowWidth="38640" windowHeight="15840" xr2:uid="{56AB0845-96B2-4058-8F7F-7188F6E2D689}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="66">
   <si>
     <t>acesso</t>
   </si>
@@ -627,20 +627,20 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -660,7 +660,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -676,9 +676,11 @@
       <c r="E2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F2" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -694,9 +696,11 @@
       <c r="E3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F3" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -716,7 +720,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -732,7 +736,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -752,7 +756,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -769,7 +773,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -790,11 +794,11 @@
       </c>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E9" s="2"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -814,7 +818,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -830,7 +834,7 @@
       <c r="F11" s="1"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -846,9 +850,11 @@
       <c r="E12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F12" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -864,9 +870,11 @@
       <c r="E13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F13" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -884,7 +892,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -898,11 +906,11 @@
         <v>32</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -916,11 +924,11 @@
         <v>33</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -940,7 +948,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -958,7 +966,7 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -976,7 +984,7 @@
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -996,7 +1004,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1016,11 +1024,11 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E22" s="2"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -1036,7 +1044,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1052,7 +1060,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1068,7 +1076,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1083,8 +1091,9 @@
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -1100,7 +1109,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -1120,7 +1129,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -1140,11 +1149,11 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E30" s="2"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -1162,7 +1171,7 @@
       </c>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -1180,7 +1189,7 @@
       </c>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -1198,23 +1207,23 @@
       </c>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E34" s="2"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E35" s="2"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E36" s="2"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E37" s="2"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F38" s="1"/>
     </row>
   </sheetData>

</xml_diff>